<commit_message>
ultime righe del dataset
</commit_message>
<xml_diff>
--- a/src/main/java/it/unisa/c07/biblionet/moduloIntelligenzaArtificiale/dataset/dataset.xlsx
+++ b/src/main/java/it/unisa/c07/biblionet/moduloIntelligenzaArtificiale/dataset/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viviana\Documents\GitHub\biblionetAI\src\main\java\it\unisa\c07\biblionet\moduloIntelligenzaArtificiale\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD90B39-E827-4B89-8FDD-F06930F0B054}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E10F3A-0F80-4560-9177-1E88CA1858C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{788EE436-A673-456E-BD35-1D95133373BC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5510" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5655" uniqueCount="150">
   <si>
     <t>Computer, programming, gaming</t>
   </si>
@@ -859,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0BAEB9-F73F-44E0-8031-860F27F46C3B}">
-  <dimension ref="A1:AC190"/>
+  <dimension ref="A1:AC195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H192" sqref="H192"/>
+    <sheetView tabSelected="1" topLeftCell="C142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,8 +890,9 @@
     <col min="23" max="23" width="19" customWidth="1"/>
     <col min="24" max="24" width="18" customWidth="1"/>
     <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="26" width="9.85546875" customWidth="1"/>
-    <col min="28" max="28" width="10.140625" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" customWidth="1"/>
     <col min="29" max="29" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17805,6 +17806,451 @@
         <v>36</v>
       </c>
     </row>
+    <row r="191" spans="1:29" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H191" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I191" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J191" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K191" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L191" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M191" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N191" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O191" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P191" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q191" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R191" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S191" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="T191" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U191" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="V191" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W191" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X191" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y191" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z191" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA191" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB191" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC191" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:29" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I192" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J192" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K192" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L192" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M192" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N192" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O192" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P192" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q192" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R192" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S192" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T192" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U192" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V192" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="W192" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X192" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y192" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z192" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA192" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB192" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC192" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="193" spans="1:29" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J193" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K193" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L193" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M193" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N193" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O193" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P193" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q193" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R193" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S193" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T193" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U193" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="V193" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W193" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X193" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y193" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z193" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA193" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB193" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC193" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="194" spans="1:29" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J194" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K194" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L194" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M194" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N194" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O194" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P194" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q194" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R194" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S194" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="T194" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U194" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V194" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="W194" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X194" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y194" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z194" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA194" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB194" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC194" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="195" spans="1:29" s="1" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J195" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K195" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L195" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M195" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N195" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O195" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P195" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q195" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R195" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S195" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T195" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U195" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="V195" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W195" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X195" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y195" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z195" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA195" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB195" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC195" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>